<commit_message>
Latest updates after adding headers to a lot of files
</commit_message>
<xml_diff>
--- a/data/xls/2009-06-01/Alcon-Jan-Jun-2009-pdf.xlsx
+++ b/data/xls/2009-06-01/Alcon-Jan-Jun-2009-pdf.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="23117"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="20" windowWidth="34200" windowHeight="22720"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060"/>
   </bookViews>
   <sheets>
     <sheet name="Table 1" sheetId="1" r:id="rId1"/>
@@ -489,15 +489,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -874,10 +868,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I104"/>
+  <dimension ref="A1:I22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:H1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -888,653 +882,483 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="26" customHeight="1">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="6" t="s">
+      <c r="B1" s="5"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="15" customHeight="1">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="10"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
     </row>
     <row r="3" spans="1:9" ht="62" customHeight="1">
-      <c r="A3" s="13" t="s">
+      <c r="A3" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="B3" s="14"/>
-      <c r="C3" s="15"/>
-      <c r="D3" s="13" t="s">
+      <c r="B3" s="12"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="13" t="s">
+      <c r="E3" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="G3" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="H3" s="5">
+      <c r="F3" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="H3" s="3">
         <v>100</v>
       </c>
-      <c r="I3" s="5" t="s">
+      <c r="I3" s="3" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="14" customHeight="1">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="10"/>
-      <c r="C4" s="11"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="12"/>
-      <c r="F4" s="12"/>
-      <c r="G4" s="12"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
+      <c r="B4" s="8"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
     </row>
     <row r="5" spans="1:9" ht="43" customHeight="1">
-      <c r="A5" s="13" t="s">
+      <c r="A5" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="14"/>
-      <c r="C5" s="15"/>
-      <c r="D5" s="13" t="s">
+      <c r="B5" s="12"/>
+      <c r="C5" s="13"/>
+      <c r="D5" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="E5" s="13" t="s">
+      <c r="E5" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="F5" s="13" t="s">
+      <c r="F5" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="G5" s="13" t="s">
+      <c r="G5" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="H5" s="5">
+      <c r="H5" s="3">
         <v>17</v>
       </c>
-      <c r="I5" s="5" t="s">
+      <c r="I5" s="3" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="46" customHeight="1">
-      <c r="A6" s="13" t="s">
+      <c r="A6" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="14"/>
-      <c r="C6" s="15"/>
-      <c r="D6" s="13" t="s">
+      <c r="B6" s="12"/>
+      <c r="C6" s="13"/>
+      <c r="D6" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="E6" s="13" t="s">
+      <c r="E6" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="F6" s="13" t="s">
+      <c r="F6" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="G6" s="13" t="s">
+      <c r="G6" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="H6" s="5">
+      <c r="H6" s="3">
         <v>37</v>
       </c>
-      <c r="I6" s="5" t="s">
+      <c r="I6" s="3" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="62" customHeight="1">
-      <c r="A7" s="13" t="s">
+      <c r="A7" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="B7" s="14"/>
-      <c r="C7" s="15"/>
-      <c r="D7" s="13" t="s">
+      <c r="B7" s="12"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="E7" s="13" t="s">
+      <c r="E7" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="F7" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="G7" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="H7" s="5">
+      <c r="F7" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="H7" s="3">
         <v>40</v>
       </c>
-      <c r="I7" s="5" t="s">
+      <c r="I7" s="3" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="18" customHeight="1">
-      <c r="A8" s="9" t="s">
+      <c r="A8" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="B8" s="10"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="12"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="4"/>
+      <c r="B8" s="8"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
     </row>
     <row r="9" spans="1:9" ht="35" customHeight="1">
-      <c r="A9" s="13" t="s">
+      <c r="A9" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="B9" s="14"/>
-      <c r="C9" s="15"/>
-      <c r="D9" s="13" t="s">
+      <c r="B9" s="12"/>
+      <c r="C9" s="13"/>
+      <c r="D9" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="E9" s="13" t="s">
+      <c r="E9" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="F9" s="13" t="s">
+      <c r="F9" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="G9" s="13" t="s">
+      <c r="G9" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="H9" s="5">
+      <c r="H9" s="3">
         <v>25</v>
       </c>
-      <c r="I9" s="5" t="s">
+      <c r="I9" s="3" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="44" customHeight="1">
-      <c r="A10" s="13" t="s">
+      <c r="A10" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="B10" s="14"/>
-      <c r="C10" s="15"/>
-      <c r="D10" s="13" t="s">
+      <c r="B10" s="12"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="E10" s="13" t="s">
+      <c r="E10" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="F10" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="G10" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="H10" s="5">
+      <c r="F10" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="G10" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="H10" s="3">
         <v>55</v>
       </c>
-      <c r="I10" s="5" t="s">
+      <c r="I10" s="3" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="53" customHeight="1">
-      <c r="A11" s="13" t="s">
+      <c r="A11" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="B11" s="14"/>
-      <c r="C11" s="15"/>
-      <c r="D11" s="13" t="s">
+      <c r="B11" s="12"/>
+      <c r="C11" s="13"/>
+      <c r="D11" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="E11" s="13" t="s">
+      <c r="E11" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="F11" s="13" t="s">
+      <c r="F11" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="G11" s="13" t="s">
+      <c r="G11" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="H11" s="5">
+      <c r="H11" s="3">
         <v>40</v>
       </c>
-      <c r="I11" s="5" t="s">
+      <c r="I11" s="3" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="86" customHeight="1">
-      <c r="A12" s="13" t="s">
+      <c r="A12" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="B12" s="14"/>
-      <c r="C12" s="15"/>
-      <c r="D12" s="13" t="s">
+      <c r="B12" s="12"/>
+      <c r="C12" s="13"/>
+      <c r="D12" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="E12" s="13" t="s">
+      <c r="E12" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="F12" s="13" t="s">
+      <c r="F12" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="G12" s="13" t="s">
+      <c r="G12" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="H12" s="5">
+      <c r="H12" s="3">
         <v>32</v>
       </c>
-      <c r="I12" s="5" t="s">
+      <c r="I12" s="3" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="13" customHeight="1">
-      <c r="A13" s="9" t="s">
+      <c r="A13" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="B13" s="10"/>
-      <c r="C13" s="11"/>
-      <c r="D13" s="12"/>
-      <c r="E13" s="12"/>
-      <c r="F13" s="12"/>
-      <c r="G13" s="12"/>
-      <c r="H13" s="4"/>
-      <c r="I13" s="4"/>
+      <c r="B13" s="8"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="10"/>
+      <c r="G13" s="10"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
     </row>
     <row r="14" spans="1:9" ht="63" customHeight="1">
-      <c r="A14" s="13" t="s">
+      <c r="A14" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="B14" s="14"/>
-      <c r="C14" s="15"/>
-      <c r="D14" s="13" t="s">
+      <c r="B14" s="12"/>
+      <c r="C14" s="13"/>
+      <c r="D14" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="E14" s="13" t="s">
+      <c r="E14" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="F14" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="G14" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="H14" s="5">
+      <c r="F14" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="G14" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="H14" s="3">
         <v>500</v>
       </c>
-      <c r="I14" s="5" t="s">
+      <c r="I14" s="3" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="15" customHeight="1">
-      <c r="A15" s="9" t="s">
+      <c r="A15" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="B15" s="10"/>
-      <c r="C15" s="11"/>
-      <c r="D15" s="12"/>
-      <c r="E15" s="12"/>
-      <c r="F15" s="12"/>
-      <c r="G15" s="12"/>
-      <c r="H15" s="4"/>
-      <c r="I15" s="4"/>
+      <c r="B15" s="8"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="10"/>
+      <c r="G15" s="10"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
     </row>
     <row r="16" spans="1:9" ht="58" customHeight="1">
-      <c r="A16" s="13" t="s">
+      <c r="A16" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="B16" s="14"/>
-      <c r="C16" s="15"/>
-      <c r="D16" s="13" t="s">
+      <c r="B16" s="12"/>
+      <c r="C16" s="13"/>
+      <c r="D16" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="E16" s="13" t="s">
+      <c r="E16" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="F16" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="G16" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="H16" s="5">
+      <c r="F16" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="G16" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="H16" s="3">
         <v>3100</v>
       </c>
-      <c r="I16" s="5" t="s">
+      <c r="I16" s="3" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="61" customHeight="1">
-      <c r="A17" s="13" t="s">
+      <c r="A17" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="B17" s="14"/>
-      <c r="C17" s="15"/>
-      <c r="D17" s="13" t="s">
+      <c r="B17" s="12"/>
+      <c r="C17" s="13"/>
+      <c r="D17" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="E17" s="13" t="s">
+      <c r="E17" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="F17" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="G17" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="H17" s="5">
+      <c r="F17" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="G17" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="H17" s="3">
         <v>250</v>
       </c>
-      <c r="I17" s="5" t="s">
+      <c r="I17" s="3" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="58" customHeight="1">
-      <c r="A18" s="13" t="s">
+      <c r="A18" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="B18" s="14"/>
-      <c r="C18" s="15"/>
-      <c r="D18" s="13" t="s">
+      <c r="B18" s="12"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="E18" s="13" t="s">
+      <c r="E18" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="F18" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="G18" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="H18" s="5">
+      <c r="F18" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="G18" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="H18" s="3">
         <v>1000</v>
       </c>
-      <c r="I18" s="5" t="s">
+      <c r="I18" s="3" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="54" customHeight="1">
-      <c r="A19" s="13" t="s">
+      <c r="A19" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="B19" s="14"/>
-      <c r="C19" s="15"/>
-      <c r="D19" s="13" t="s">
+      <c r="B19" s="12"/>
+      <c r="C19" s="13"/>
+      <c r="D19" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="E19" s="13" t="s">
+      <c r="E19" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="F19" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="G19" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="H19" s="5">
+      <c r="F19" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="G19" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="H19" s="3">
         <v>300</v>
       </c>
-      <c r="I19" s="5" t="s">
+      <c r="I19" s="3" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="18" customHeight="1">
-      <c r="A20" s="9" t="s">
+      <c r="A20" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="B20" s="10"/>
-      <c r="C20" s="11"/>
-      <c r="D20" s="12"/>
-      <c r="E20" s="12"/>
-      <c r="F20" s="12"/>
-      <c r="G20" s="12"/>
-      <c r="H20" s="4"/>
-      <c r="I20" s="4"/>
+      <c r="B20" s="8"/>
+      <c r="C20" s="9"/>
+      <c r="D20" s="10"/>
+      <c r="E20" s="10"/>
+      <c r="F20" s="10"/>
+      <c r="G20" s="10"/>
+      <c r="H20" s="2"/>
+      <c r="I20" s="2"/>
     </row>
     <row r="21" spans="1:9" ht="57" customHeight="1">
-      <c r="A21" s="13" t="s">
+      <c r="A21" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="B21" s="14"/>
-      <c r="C21" s="15"/>
-      <c r="D21" s="13" t="s">
+      <c r="B21" s="12"/>
+      <c r="C21" s="13"/>
+      <c r="D21" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="E21" s="13" t="s">
+      <c r="E21" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="F21" s="13" t="s">
+      <c r="F21" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="G21" s="13" t="s">
+      <c r="G21" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="H21" s="5">
+      <c r="H21" s="3">
         <v>50</v>
       </c>
-      <c r="I21" s="5" t="s">
+      <c r="I21" s="3" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="87" customHeight="1">
-      <c r="A22" s="13" t="s">
+      <c r="A22" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="B22" s="14"/>
-      <c r="C22" s="15"/>
-      <c r="D22" s="13" t="s">
+      <c r="B22" s="12"/>
+      <c r="C22" s="13"/>
+      <c r="D22" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="E22" s="13" t="s">
+      <c r="E22" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="F22" s="13" t="s">
+      <c r="F22" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="G22" s="13" t="s">
+      <c r="G22" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="H22" s="5">
+      <c r="H22" s="3">
         <v>11</v>
       </c>
-      <c r="I22" s="5" t="s">
+      <c r="I22" s="3" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="9" customHeight="1">
-      <c r="A23" s="13"/>
-      <c r="B23" s="14"/>
-      <c r="C23" s="15"/>
-      <c r="D23" s="13"/>
-      <c r="E23" s="13"/>
-      <c r="F23" s="13"/>
-      <c r="G23" s="13"/>
-      <c r="H23" s="5"/>
-      <c r="I23" s="5"/>
-    </row>
-    <row r="24" spans="1:9" ht="9" customHeight="1">
-      <c r="A24" s="13"/>
-      <c r="B24" s="14"/>
-      <c r="C24" s="15"/>
-      <c r="D24" s="13"/>
-      <c r="E24" s="13"/>
-      <c r="F24" s="13"/>
-      <c r="G24" s="13"/>
-      <c r="H24" s="5"/>
-      <c r="I24" s="5"/>
-    </row>
-    <row r="25" spans="1:9" ht="9" customHeight="1">
-      <c r="A25" s="13"/>
-      <c r="B25" s="14"/>
-      <c r="C25" s="15"/>
-      <c r="D25" s="13"/>
-      <c r="E25" s="13"/>
-      <c r="F25" s="13"/>
-      <c r="G25" s="13"/>
-      <c r="H25" s="5"/>
-      <c r="I25" s="5"/>
-    </row>
-    <row r="26" spans="1:9" ht="10" customHeight="1"/>
-    <row r="27" spans="1:9" ht="9" customHeight="1"/>
-    <row r="28" spans="1:9" ht="10" customHeight="1"/>
-    <row r="29" spans="1:9" ht="10" customHeight="1"/>
-    <row r="30" spans="1:9" ht="9" customHeight="1"/>
-    <row r="31" spans="1:9" ht="9" customHeight="1"/>
-    <row r="32" spans="1:9" ht="10" customHeight="1"/>
-    <row r="33" spans="1:1" ht="9" customHeight="1"/>
-    <row r="34" spans="1:1" ht="9" customHeight="1"/>
-    <row r="35" spans="1:1" ht="9" customHeight="1"/>
-    <row r="36" spans="1:1" ht="9" customHeight="1"/>
-    <row r="37" spans="1:1" ht="9" customHeight="1">
-      <c r="A37" s="1"/>
-    </row>
-    <row r="38" spans="1:1" ht="9" customHeight="1">
-      <c r="A38" s="1"/>
-    </row>
-    <row r="39" spans="1:1" ht="9" customHeight="1"/>
-    <row r="40" spans="1:1" ht="9" customHeight="1"/>
-    <row r="41" spans="1:1" ht="9" customHeight="1"/>
-    <row r="42" spans="1:1" ht="9" customHeight="1"/>
-    <row r="43" spans="1:1" ht="9" customHeight="1"/>
-    <row r="44" spans="1:1" ht="10" customHeight="1"/>
-    <row r="45" spans="1:1" ht="10" customHeight="1"/>
-    <row r="46" spans="1:1" ht="9" customHeight="1"/>
-    <row r="47" spans="1:1" ht="9" customHeight="1"/>
-    <row r="48" spans="1:1" ht="9" customHeight="1">
-      <c r="A48" s="1"/>
-    </row>
-    <row r="49" spans="1:1" ht="9" customHeight="1"/>
-    <row r="50" spans="1:1" ht="10" customHeight="1"/>
-    <row r="51" spans="1:1" ht="9" customHeight="1"/>
-    <row r="52" spans="1:1" ht="9" customHeight="1"/>
-    <row r="53" spans="1:1" ht="9" customHeight="1"/>
-    <row r="54" spans="1:1" ht="9" customHeight="1"/>
-    <row r="55" spans="1:1" ht="9" customHeight="1"/>
-    <row r="56" spans="1:1" ht="9" customHeight="1"/>
-    <row r="57" spans="1:1" ht="9" customHeight="1">
-      <c r="A57" s="1"/>
-    </row>
-    <row r="58" spans="1:1" ht="9" customHeight="1">
-      <c r="A58" s="1"/>
-    </row>
-    <row r="59" spans="1:1" ht="9" customHeight="1">
-      <c r="A59" s="1"/>
-    </row>
-    <row r="60" spans="1:1" ht="9" customHeight="1"/>
-    <row r="61" spans="1:1" ht="9" customHeight="1"/>
-    <row r="62" spans="1:1" ht="9" customHeight="1">
-      <c r="A62" s="1"/>
-    </row>
-    <row r="63" spans="1:1" ht="9" customHeight="1">
-      <c r="A63" s="1"/>
-    </row>
-    <row r="64" spans="1:1" ht="9" customHeight="1">
-      <c r="A64" s="1"/>
-    </row>
-    <row r="65" spans="1:1" ht="9" customHeight="1">
-      <c r="A65" s="1"/>
-    </row>
-    <row r="66" spans="1:1" ht="9" customHeight="1"/>
-    <row r="67" spans="1:1" ht="10" customHeight="1"/>
-    <row r="68" spans="1:1" ht="9" customHeight="1"/>
-    <row r="69" spans="1:1" ht="10" customHeight="1"/>
-    <row r="70" spans="1:1" ht="10" customHeight="1"/>
-    <row r="71" spans="1:1" ht="10" customHeight="1"/>
-    <row r="72" spans="1:1" ht="10" customHeight="1">
-      <c r="A72" s="1"/>
-    </row>
-    <row r="73" spans="1:1" ht="10" customHeight="1">
-      <c r="A73" s="1"/>
-    </row>
-    <row r="74" spans="1:1" ht="10" customHeight="1">
-      <c r="A74" s="1"/>
-    </row>
-    <row r="75" spans="1:1" ht="10" customHeight="1">
-      <c r="A75" s="1"/>
-    </row>
-    <row r="76" spans="1:1" ht="10" customHeight="1">
-      <c r="A76" s="1"/>
-    </row>
-    <row r="77" spans="1:1" ht="10" customHeight="1">
-      <c r="A77" s="2"/>
-    </row>
-    <row r="78" spans="1:1" ht="10" customHeight="1">
-      <c r="A78" s="2"/>
-    </row>
-    <row r="79" spans="1:1" ht="10" customHeight="1"/>
-    <row r="80" spans="1:1" ht="10" customHeight="1"/>
-    <row r="81" spans="1:1" ht="10" customHeight="1"/>
-    <row r="82" spans="1:1" ht="10" customHeight="1">
-      <c r="A82" s="1"/>
-    </row>
-    <row r="83" spans="1:1" ht="10" customHeight="1">
-      <c r="A83" s="1"/>
-    </row>
-    <row r="84" spans="1:1" ht="10" customHeight="1">
-      <c r="A84" s="1"/>
-    </row>
-    <row r="85" spans="1:1" ht="10" customHeight="1">
-      <c r="A85" s="1"/>
-    </row>
-    <row r="86" spans="1:1" ht="10" customHeight="1"/>
-    <row r="87" spans="1:1" ht="10" customHeight="1">
-      <c r="A87" s="1"/>
-    </row>
-    <row r="88" spans="1:1" ht="10" customHeight="1">
-      <c r="A88" s="1"/>
-    </row>
-    <row r="89" spans="1:1" ht="10" customHeight="1">
-      <c r="A89" s="1"/>
-    </row>
-    <row r="90" spans="1:1" ht="9" customHeight="1"/>
-    <row r="91" spans="1:1" ht="9" customHeight="1">
-      <c r="A91" s="1"/>
-    </row>
-    <row r="92" spans="1:1" ht="9" customHeight="1">
-      <c r="A92" s="1"/>
-    </row>
-    <row r="93" spans="1:1" ht="9" customHeight="1">
-      <c r="A93" s="1"/>
-    </row>
-    <row r="94" spans="1:1" ht="9" customHeight="1">
-      <c r="A94" s="1"/>
-    </row>
-    <row r="95" spans="1:1" ht="9" customHeight="1">
-      <c r="A95" s="1"/>
-    </row>
-    <row r="96" spans="1:1" ht="9" customHeight="1"/>
-    <row r="97" ht="9" customHeight="1"/>
-    <row r="98" ht="9" customHeight="1"/>
-    <row r="99" ht="9" customHeight="1"/>
-    <row r="100" ht="9" customHeight="1"/>
-    <row r="101" ht="9" customHeight="1"/>
-    <row r="102" ht="9" customHeight="1"/>
-    <row r="103" ht="18" customHeight="1"/>
-    <row r="104" ht="9" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>